<commit_message>
Pygame muziek en icon
</commit_message>
<xml_diff>
--- a/vragenlijst.xlsx
+++ b/vragenlijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niels\OneDrive\Documenten\Programming\School\Sorteerhoed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7B6211-161E-4F25-9E49-9831DD1EC8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6F2C4D-F597-481B-9601-48B4E90DF7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
   <si>
     <t>vraag</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Zoeken wie het heeft gedaan en vragen of zij het terug kunnen draaien.</t>
   </si>
   <si>
-    <t>In welk onderdeel van de magische wereld van Hogwarts ben jij het meest geïntereseerd?</t>
-  </si>
-  <si>
     <t>In duistere magie?</t>
   </si>
   <si>
@@ -109,16 +106,206 @@
   </si>
   <si>
     <t>Wachter(De drie ringen verdedigen van de jagers die willen scoren)</t>
+  </si>
+  <si>
+    <t>In welk onderdeel van de magische wereld van Hogwarts ben jij het meest geïnteresseerd?</t>
+  </si>
+  <si>
+    <t>Hoe wil je gaan voor de winst?</t>
+  </si>
+  <si>
+    <t>Inspelen op de zwakke punten van de tegenstander?</t>
+  </si>
+  <si>
+    <t>Zoveel mogelijk doelpunten scoren om zo tijd te winnen voor de zoeker?</t>
+  </si>
+  <si>
+    <t>Zo snel mogelijk de snitch pakken?</t>
+  </si>
+  <si>
+    <t>Zorgen dat de topspelers van de tegenstander eruit worden gespeeld door de drijvers?</t>
+  </si>
+  <si>
+    <t>Waar zoek jij je avontuur in Hogwarts?</t>
+  </si>
+  <si>
+    <t>De mysteries opzoeken in het verboden bos?</t>
+  </si>
+  <si>
+    <t>De meest vreemde potions bedenken in de Potion classroom?</t>
+  </si>
+  <si>
+    <t>Te weten komen over spreueken en geschiedenis in de library?</t>
+  </si>
+  <si>
+    <t>Of begkijk je graag de zwerkbal wedstrijden?</t>
+  </si>
+  <si>
+    <t>Stel je krijgt een potion voorgeschoteld die jij moet na brouwen, hoe ga je hiermee aan de slag?</t>
+  </si>
+  <si>
+    <t>Je onderzoekt de potion doorgrondig om zo alle ingrediënten te achterhalen.</t>
+  </si>
+  <si>
+    <t>Je gooit random ingrediënten bij elkaar en hoopt dat je het in 1x goed krijgt.</t>
+  </si>
+  <si>
+    <t>Via trial en error proberen achter de ingrediënten te komen.</t>
+  </si>
+  <si>
+    <t>Je verzamelt van alle andere opties de uitkomst en gebruikt die informatie om de potion te maken.</t>
+  </si>
+  <si>
+    <t>De headmaster heeft je staf afgenomen, hoe krijg je je staf weer terug?</t>
+  </si>
+  <si>
+    <t>Kijken of je een back=up hebt, zo niet dan terughaalsoftware gebruiken of schijven restoren.</t>
+  </si>
+  <si>
+    <t>Bedenk een oplossing om je staf weer terug te pakken. (Bijvoorbeeld jezelf onzichtbaar maken en zo in het kantoor je staf terugpakken) </t>
+  </si>
+  <si>
+    <t>Analyseert de mogelijkeden hoe ze hem terug kunnen krijgen op de beste manier en gebruiken de best practice.</t>
+  </si>
+  <si>
+    <t>Wachten tot je je staf krijgt en in de tussentijd werken met een leenstaf</t>
+  </si>
+  <si>
+    <t>Stel je hebt een curse gekregen van de duistere magie, wat zou je doen om de curse van je af te halen? </t>
+  </si>
+  <si>
+    <t>Ik weet zelf hoe ik dit van mezelf moet afhalen, geef me maar deze ingrediënten en ik los het wel op. </t>
+  </si>
+  <si>
+    <t>Je ziet de curse in als een raadsel die je gaat proberen op te lossen.</t>
+  </si>
+  <si>
+    <t>Ga naar de leraar toe en vraag om hulp omdat je het niet weet.</t>
+  </si>
+  <si>
+    <t>In je boeken over duistere magie zoeken naar de curse die je hebt en hoe je ervan afkomt.</t>
+  </si>
+  <si>
+    <t>Een vriend van je is erachter gekomen hoe je onzichtbaar kan worden, jij wilt dit ook kunnen alleen die vriend verteld dit niet aan je, hoe los je dit op?</t>
+  </si>
+  <si>
+    <t>Alle bronnen van diegene onderzoeken naar informatie die kan leiden tot dit geheim.</t>
+  </si>
+  <si>
+    <t>Proberen op alternatieve manieren om onzichtbaar te worden.</t>
+  </si>
+  <si>
+    <t>Ga naar de library en zoek naar een boek over onzichtbaarheid.</t>
+  </si>
+  <si>
+    <t>Analyseer alle mogelijkheden die je vriend heeft kunnen gebruiken en probeer het op de manier te doen waarop je vriend het heeft kunnen doen. </t>
+  </si>
+  <si>
+    <t>Hoe kom je erachter wat de vloek des doods is?</t>
+  </si>
+  <si>
+    <t>Je hebt er in het verleden over gehoord en probeert contact op te zoeken met diegene die het je al heeft verteld.</t>
+  </si>
+  <si>
+    <t>Je maakt jezelf onzichtbaar om in de verboden afdeling van de library te gaan.</t>
+  </si>
+  <si>
+    <t>Je wilt dit niet eens weten, want het spreekt je niet aan.</t>
+  </si>
+  <si>
+    <t>Je gaat op zoek naar boeken in de library die er van alles over vertellen om een beeld te creëren wat het met je kan doen.</t>
+  </si>
+  <si>
+    <t>Je bent in de bibliotheek, naar wat voor boek zoek je?</t>
+  </si>
+  <si>
+    <t>‘The mysteries of the forbidden forest volume I’ </t>
+  </si>
+  <si>
+    <t>‘How to craft a broom 101’</t>
+  </si>
+  <si>
+    <t>‘The art of creating spells volume I’</t>
+  </si>
+  <si>
+    <t>‘The greatest quidditch matches of alltime volume I’</t>
+  </si>
+  <si>
+    <t>Stel je hebt vrije loop in het verboden bos, wat ga je doen?</t>
+  </si>
+  <si>
+    <t>Je gaat dieper het bos in om te vinden wat er zo verboden aan is.</t>
+  </si>
+  <si>
+    <t>Je zoekt inspiratie voor een duister verhaal dat je aan het schrijven bent.</t>
+  </si>
+  <si>
+    <t>Je zoekt je weg naar buiten want je bent bang.</t>
+  </si>
+  <si>
+    <t>Je gaat opzoek naar de monsters waarover je hebt gehoord.</t>
+  </si>
+  <si>
+    <t>Je komt per ongeluk voor de deur te staan waar je vanaf het begin van het jaar niet naar binnen mag, wat doe je?</t>
+  </si>
+  <si>
+    <t>Je opent simpelweg de deur en kijkt wat erachter staat.</t>
+  </si>
+  <si>
+    <t>Je zoekt naar een oplossing om van buitenaf naar binnen te kijken (met een spreuk of met een magisch voorwerp bijv.)</t>
+  </si>
+  <si>
+    <t>Je gaat door het sleutelgat kijken wat erachter zit, omdat je toch best nieuwsgierig bent.</t>
+  </si>
+  <si>
+    <t>Bekijkt de mogelijkheden die er zijn en brengt dit in kaart.</t>
+  </si>
+  <si>
+    <t>Je ziet iemand een spell uitvoeren, je ziet dat de kleur een blauwe flair heeft, hoe zou je achterhalen hoe de flair blauw is?</t>
+  </si>
+  <si>
+    <t>Je kan uitzoeken welke benodigdheden je nodig hebt om de de spel tot stand te krijgen, dit vervolgens noteren en rapport voor uitdraaien.</t>
+  </si>
+  <si>
+    <t>De kleur blauw spreekt je niet aan dus je gaat proberen spells te maken met een andere flair dan blauw.</t>
+  </si>
+  <si>
+    <t>Je zoekt die specifieke spell en achterhaalt daaruit wat de flair blauw maakt.</t>
+  </si>
+  <si>
+    <t>Je kijkt naar andere spells met een blauwe flair en probeer dit te reproduceren.</t>
+  </si>
+  <si>
+    <t>Je spreekt per ongeluk de naam uit van degene “Waarvan de naam niet mag worden genoemd uit”, wat doe je?</t>
+  </si>
+  <si>
+    <t>Je wacht af wat er gebeurt en je loopt rustig verder.</t>
+  </si>
+  <si>
+    <t>Kan kijken naar het gevolg en proberen hierop in te spelen</t>
+  </si>
+  <si>
+    <t>Ik bouw een muur om mij heen en isoleer mij van de buitenwereld.</t>
+  </si>
+  <si>
+    <t>Je geeft op omdat het de afgelopen keren ook in de dood is afgelopen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,8 +331,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +617,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,19 +692,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -533,20 +721,20 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -561,6 +749,21 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
@@ -575,6 +778,21 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
@@ -589,6 +807,21 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
@@ -603,6 +836,21 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
@@ -617,6 +865,21 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
@@ -631,6 +894,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
@@ -645,6 +923,21 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
@@ -659,6 +952,21 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
@@ -673,6 +981,21 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
@@ -687,6 +1010,21 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
@@ -701,6 +1039,21 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
@@ -715,6 +1068,21 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
       <c r="F16" t="s">
         <v>10</v>
       </c>
@@ -730,5 +1098,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>